<commit_message>
RCI BRIEF values and other pre/post data added
</commit_message>
<xml_diff>
--- a/data/GIAD_brief.xlsx
+++ b/data/GIAD_brief.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/aaron_pilot_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4472CD0-2960-4C42-AF5E-A00395B382F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7107FA-51A8-CA44-A3BE-527043A4118B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15660" xr2:uid="{11F1717A-72AE-CB42-AE29-0C1B97B79501}"/>
+    <workbookView xWindow="-21640" yWindow="-18000" windowWidth="27640" windowHeight="15660" xr2:uid="{11F1717A-72AE-CB42-AE29-0C1B97B79501}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Scale/Index</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Percentile Rank Post</t>
+  </si>
+  <si>
+    <t>RCI</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254E6158-84C2-8145-A20F-81A65778F7B7}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -449,9 +452,10 @@
     <col min="3" max="3" width="17.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +471,11 @@
       <c r="E1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -484,8 +491,11 @@
       <c r="E2">
         <v>41</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -501,8 +511,11 @@
       <c r="E3">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3">
+        <v>-1.83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -518,8 +531,11 @@
       <c r="E4">
         <v>52</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -535,8 +551,11 @@
       <c r="E5">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -552,8 +571,11 @@
       <c r="E6">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -569,8 +591,11 @@
       <c r="E7">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -586,8 +611,11 @@
       <c r="E8">
         <v>70</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -603,8 +631,11 @@
       <c r="E9">
         <v>41</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9">
+        <v>-0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -620,8 +651,11 @@
       <c r="E10">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10">
+        <v>-1.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -637,8 +671,11 @@
       <c r="E11">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -654,8 +691,11 @@
       <c r="E12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12">
+        <v>-1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -670,6 +710,9 @@
       </c>
       <c r="E13">
         <v>22</v>
+      </c>
+      <c r="F13">
+        <v>-0.31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>